<commit_message>
Removed extraneous rmd file
</commit_message>
<xml_diff>
--- a/Act_135_Philly/raw/discrepancies.xlsx
+++ b/Act_135_Philly/raw/discrepancies.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26903"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{37DD63B6-87A3-4804-9205-2E4A189D8B91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ejs/Documents/GitHub/Act-135/Act_135_Philly/raw/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16F66E18-18F4-5048-9622-A01FCCA76C8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="620" yWindow="640" windowWidth="28800" windowHeight="16360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="discrepancies" sheetId="1" r:id="rId1"/>
@@ -31,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="112">
   <si>
     <t>respondent</t>
   </si>
@@ -313,13 +318,67 @@
   </si>
   <si>
     <t>CAVE</t>
+  </si>
+  <si>
+    <t>AURORA</t>
+  </si>
+  <si>
+    <t>VALENTINE</t>
+  </si>
+  <si>
+    <t>ANGEL</t>
+  </si>
+  <si>
+    <t>RODRIGUEZ</t>
+  </si>
+  <si>
+    <t>SAMUEL WILMER</t>
+  </si>
+  <si>
+    <t>HARRIS</t>
+  </si>
+  <si>
+    <t>JAMES</t>
+  </si>
+  <si>
+    <t>EDWARD</t>
+  </si>
+  <si>
+    <t>EPURE</t>
+  </si>
+  <si>
+    <t>ZEOLA</t>
+  </si>
+  <si>
+    <t>LANCASTER</t>
+  </si>
+  <si>
+    <t>RUDOLPH</t>
+  </si>
+  <si>
+    <t>POLSELLI</t>
+  </si>
+  <si>
+    <t>JEFFIE</t>
+  </si>
+  <si>
+    <t>SHERFON</t>
+  </si>
+  <si>
+    <t>MCNAIR</t>
+  </si>
+  <si>
+    <t>MAMIE</t>
+  </si>
+  <si>
+    <t>COOK</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -331,12 +390,14 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -588,20 +649,21 @@
   <dimension ref="A1:H41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I36" sqref="I36:I44"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="109.7109375" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" style="5" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" customWidth="1"/>
+    <col min="1" max="1" width="109.6640625" customWidth="1"/>
+    <col min="2" max="2" width="12.5" style="5" customWidth="1"/>
+    <col min="3" max="3" width="12.5" customWidth="1"/>
     <col min="4" max="4" width="6" customWidth="1"/>
-    <col min="5" max="5" width="6.85546875" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" customWidth="1"/>
+    <col min="6" max="6" width="28.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -627,7 +689,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -653,7 +715,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
@@ -679,7 +741,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>18</v>
       </c>
@@ -705,7 +767,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>21</v>
       </c>
@@ -731,7 +793,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>24</v>
       </c>
@@ -757,7 +819,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>27</v>
       </c>
@@ -783,7 +845,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>30</v>
       </c>
@@ -809,7 +871,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>33</v>
       </c>
@@ -835,7 +897,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>36</v>
       </c>
@@ -861,7 +923,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>39</v>
       </c>
@@ -887,7 +949,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="2" t="s">
         <v>43</v>
       </c>
@@ -913,7 +975,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="2" t="s">
         <v>46</v>
       </c>
@@ -939,7 +1001,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="2" t="s">
         <v>49</v>
       </c>
@@ -965,7 +1027,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="2" t="s">
         <v>52</v>
       </c>
@@ -991,7 +1053,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="2" t="s">
         <v>55</v>
       </c>
@@ -1017,7 +1079,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="2" t="s">
         <v>58</v>
       </c>
@@ -1037,7 +1099,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="2" t="s">
         <v>61</v>
       </c>
@@ -1057,7 +1119,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="2" t="s">
         <v>62</v>
       </c>
@@ -1077,7 +1139,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="2" t="s">
         <v>63</v>
       </c>
@@ -1097,7 +1159,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="2" t="s">
         <v>64</v>
       </c>
@@ -1117,7 +1179,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="2" t="s">
         <v>65</v>
       </c>
@@ -1137,7 +1199,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="2" t="s">
         <v>66</v>
       </c>
@@ -1157,7 +1219,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="2" t="s">
         <v>67</v>
       </c>
@@ -1177,7 +1239,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="2" t="s">
         <v>68</v>
       </c>
@@ -1196,8 +1258,14 @@
       <c r="F25" s="2" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="26" spans="1:6">
+      <c r="G25" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="2" t="s">
         <v>68</v>
       </c>
@@ -1216,8 +1284,14 @@
       <c r="F26" s="2" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="27" spans="1:6">
+      <c r="G26" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="2" t="s">
         <v>71</v>
       </c>
@@ -1236,8 +1310,14 @@
       <c r="F27" s="2" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="28" spans="1:6">
+      <c r="G27" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="2" t="s">
         <v>72</v>
       </c>
@@ -1256,8 +1336,14 @@
       <c r="F28" s="2" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="29" spans="1:6">
+      <c r="G28" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="2" t="s">
         <v>73</v>
       </c>
@@ -1276,8 +1362,14 @@
       <c r="F29" s="2" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="30" spans="1:6">
+      <c r="G29" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="2" t="s">
         <v>74</v>
       </c>
@@ -1296,8 +1388,14 @@
       <c r="F30" s="2" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="31" spans="1:6">
+      <c r="G30" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="2" t="s">
         <v>73</v>
       </c>
@@ -1316,8 +1414,14 @@
       <c r="F31" s="2" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="32" spans="1:6">
+      <c r="G31" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="2" t="s">
         <v>75</v>
       </c>
@@ -1336,8 +1440,14 @@
       <c r="F32" s="2" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="33" spans="1:8">
+      <c r="G32" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="2" t="s">
         <v>76</v>
       </c>
@@ -1356,8 +1466,14 @@
       <c r="F33" s="2" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="34" spans="1:8">
+      <c r="G33" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="2" t="s">
         <v>77</v>
       </c>
@@ -1376,8 +1492,14 @@
       <c r="F34" s="2" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="35" spans="1:8">
+      <c r="G34" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="2" t="s">
         <v>78</v>
       </c>
@@ -1396,8 +1518,14 @@
       <c r="F35" s="2" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="36" spans="1:8">
+      <c r="G35" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="2" t="s">
         <v>79</v>
       </c>
@@ -1416,8 +1544,14 @@
       <c r="F36" s="2" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="37" spans="1:8">
+      <c r="G36" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="2" t="s">
         <v>80</v>
       </c>
@@ -1443,7 +1577,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="2" t="s">
         <v>85</v>
       </c>
@@ -1469,7 +1603,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="2" t="s">
         <v>88</v>
       </c>
@@ -1495,7 +1629,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="2" t="s">
         <v>80</v>
       </c>
@@ -1521,7 +1655,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="2" t="s">
         <v>91</v>
       </c>

</xml_diff>